<commit_message>
update Gibraltar com typologies 50:50 CDL/CDN
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
+++ b/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFF583B-EF5C-1F46-B7DC-B09CF39B435A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20520" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,10 +31,14 @@
     <t>Hotels</t>
   </si>
   <si>
-    <t>3.6% CR/LFM+CDL/H:1/Offices
-9.1% CR/LFM+CDL/H:2/Offices
-21.8% CR/LFM+CDL/HBET:3-5/Offices
-1.8% CR/LFM+CDL/HBET:6-/Offices
+    <t>1.8% CR/LFM+CDN/H:1/Offices
+4.55% CR/LFM+CDN/H:2/Offices
+10.9% CR/LFM+CDN/HBET:3-5/Offices
+0.9% CR/LFM+CDN/HBET:6-/Offices
+1.8% CR/LFM+CDL/H:1/Offices
+4.55% CR/LFM+CDL/H:2/Offices
+10.9% CR/LFM+CDL/HBET:3-5/Offices
+0.9% CR/LFM+CDL/HBET:6-/Offices
 3.6% MR/LWAL+CDL/H:1/Offices
 7.3% MR/LWAL+CDL/H:2/Offices
 25.5% MR/LWAL+CDL/HBET:3-5/Offices
@@ -44,8 +54,10 @@
 0.0% W/LFM+CDL/H:2/Offices</t>
   </si>
   <si>
-    <t>16.4% CR/LFM+CDL/H:1/Trade
-1.8% CR/LFM+CDL/H:2/Trade
+    <t>8.2% CR/LFM+CDL/H:1/Trade
+0.9% CR/LFM+CDL/H:2/Trade
+8.2% CR/LFM+CDL/H:1/Trade
+0.9% CR/LFM+CDL/H:2/Trade
 0.0% CR/LFM+CDL/HBET:3-5/Trade
 0.0% CR/LFM+CDL/HBET:6-/Trade
 32.7% MR/LWAL+CDL/H:1/Trade
@@ -63,10 +75,14 @@
 0.4% W/LFM+CDL/H:2/Trade</t>
   </si>
   <si>
-    <t>4.4% CR/LFM+CDL/H:1/Hotels
- 1.8% CR/LFM+CDL/H:2/Hotels
- 10.6% CR/LFM+CDL/HBET:3-5/Hotels
- 0.9% CR/LFM+CDL/HBET:6-/Hotels
+    <t>2.2% CR/LFM+CDN/H:1/Hotels
+0.9% CR/LFM+CDN/H:2/Hotels
+5.3% CR/LFM+CDN/HBET:3-5/Hotels
+0.45% CR/LFM+CDN/HBET:6-/Hotels
+2.2% CR/LFM+CDL/H:1/Hotels
+0.9% CR/LFM+CDL/H:2/Hotels
+5.3% CR/LFM+CDL/HBET:3-5/Hotels
+0.45% CR/LFM+CDL/HBET:6-/Hotels
  3.5% MR/LWAL+CDL/H:1/Hotels
  7.1% MR/LWAL+CDL/H:2/Hotels
  25.1% MR/LWAL+CDL/HBET:3-5/Hotels
@@ -85,8 +101,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,10 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,6 +168,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -195,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,9 +254,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,6 +306,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,14 +499,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,14 +524,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="335" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "update Gibraltar com typologies 50:50 CDL/CDN"
This reverts commit 0565b11dbb0921d605a3f20ca7fa9c9c46a57dce.
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
+++ b/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFF583B-EF5C-1F46-B7DC-B09CF39B435A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20520" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -31,14 +25,10 @@
     <t>Hotels</t>
   </si>
   <si>
-    <t>1.8% CR/LFM+CDN/H:1/Offices
-4.55% CR/LFM+CDN/H:2/Offices
-10.9% CR/LFM+CDN/HBET:3-5/Offices
-0.9% CR/LFM+CDN/HBET:6-/Offices
-1.8% CR/LFM+CDL/H:1/Offices
-4.55% CR/LFM+CDL/H:2/Offices
-10.9% CR/LFM+CDL/HBET:3-5/Offices
-0.9% CR/LFM+CDL/HBET:6-/Offices
+    <t>3.6% CR/LFM+CDL/H:1/Offices
+9.1% CR/LFM+CDL/H:2/Offices
+21.8% CR/LFM+CDL/HBET:3-5/Offices
+1.8% CR/LFM+CDL/HBET:6-/Offices
 3.6% MR/LWAL+CDL/H:1/Offices
 7.3% MR/LWAL+CDL/H:2/Offices
 25.5% MR/LWAL+CDL/HBET:3-5/Offices
@@ -54,10 +44,8 @@
 0.0% W/LFM+CDL/H:2/Offices</t>
   </si>
   <si>
-    <t>8.2% CR/LFM+CDL/H:1/Trade
-0.9% CR/LFM+CDL/H:2/Trade
-8.2% CR/LFM+CDL/H:1/Trade
-0.9% CR/LFM+CDL/H:2/Trade
+    <t>16.4% CR/LFM+CDL/H:1/Trade
+1.8% CR/LFM+CDL/H:2/Trade
 0.0% CR/LFM+CDL/HBET:3-5/Trade
 0.0% CR/LFM+CDL/HBET:6-/Trade
 32.7% MR/LWAL+CDL/H:1/Trade
@@ -75,14 +63,10 @@
 0.4% W/LFM+CDL/H:2/Trade</t>
   </si>
   <si>
-    <t>2.2% CR/LFM+CDN/H:1/Hotels
-0.9% CR/LFM+CDN/H:2/Hotels
-5.3% CR/LFM+CDN/HBET:3-5/Hotels
-0.45% CR/LFM+CDN/HBET:6-/Hotels
-2.2% CR/LFM+CDL/H:1/Hotels
-0.9% CR/LFM+CDL/H:2/Hotels
-5.3% CR/LFM+CDL/HBET:3-5/Hotels
-0.45% CR/LFM+CDL/HBET:6-/Hotels
+    <t>4.4% CR/LFM+CDL/H:1/Hotels
+ 1.8% CR/LFM+CDL/H:2/Hotels
+ 10.6% CR/LFM+CDL/HBET:3-5/Hotels
+ 0.9% CR/LFM+CDL/HBET:6-/Hotels
  3.5% MR/LWAL+CDL/H:1/Hotels
  7.1% MR/LWAL+CDL/H:2/Hotels
  25.1% MR/LWAL+CDL/HBET:3-5/Hotels
@@ -101,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,13 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -168,14 +149,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -222,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,27 +227,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,24 +261,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,21 +436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,14 +454,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="335" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "update Gibraltar com typologies 50:50 CDL/CDN""
This reverts commit 86933f3f2085f7426d6e863acdaed808aa3ea5cb.
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
+++ b/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFF583B-EF5C-1F46-B7DC-B09CF39B435A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20520" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,10 +31,14 @@
     <t>Hotels</t>
   </si>
   <si>
-    <t>3.6% CR/LFM+CDL/H:1/Offices
-9.1% CR/LFM+CDL/H:2/Offices
-21.8% CR/LFM+CDL/HBET:3-5/Offices
-1.8% CR/LFM+CDL/HBET:6-/Offices
+    <t>1.8% CR/LFM+CDN/H:1/Offices
+4.55% CR/LFM+CDN/H:2/Offices
+10.9% CR/LFM+CDN/HBET:3-5/Offices
+0.9% CR/LFM+CDN/HBET:6-/Offices
+1.8% CR/LFM+CDL/H:1/Offices
+4.55% CR/LFM+CDL/H:2/Offices
+10.9% CR/LFM+CDL/HBET:3-5/Offices
+0.9% CR/LFM+CDL/HBET:6-/Offices
 3.6% MR/LWAL+CDL/H:1/Offices
 7.3% MR/LWAL+CDL/H:2/Offices
 25.5% MR/LWAL+CDL/HBET:3-5/Offices
@@ -44,8 +54,10 @@
 0.0% W/LFM+CDL/H:2/Offices</t>
   </si>
   <si>
-    <t>16.4% CR/LFM+CDL/H:1/Trade
-1.8% CR/LFM+CDL/H:2/Trade
+    <t>8.2% CR/LFM+CDL/H:1/Trade
+0.9% CR/LFM+CDL/H:2/Trade
+8.2% CR/LFM+CDL/H:1/Trade
+0.9% CR/LFM+CDL/H:2/Trade
 0.0% CR/LFM+CDL/HBET:3-5/Trade
 0.0% CR/LFM+CDL/HBET:6-/Trade
 32.7% MR/LWAL+CDL/H:1/Trade
@@ -63,10 +75,14 @@
 0.4% W/LFM+CDL/H:2/Trade</t>
   </si>
   <si>
-    <t>4.4% CR/LFM+CDL/H:1/Hotels
- 1.8% CR/LFM+CDL/H:2/Hotels
- 10.6% CR/LFM+CDL/HBET:3-5/Hotels
- 0.9% CR/LFM+CDL/HBET:6-/Hotels
+    <t>2.2% CR/LFM+CDN/H:1/Hotels
+0.9% CR/LFM+CDN/H:2/Hotels
+5.3% CR/LFM+CDN/HBET:3-5/Hotels
+0.45% CR/LFM+CDN/HBET:6-/Hotels
+2.2% CR/LFM+CDL/H:1/Hotels
+0.9% CR/LFM+CDL/H:2/Hotels
+5.3% CR/LFM+CDL/HBET:3-5/Hotels
+0.45% CR/LFM+CDL/HBET:6-/Hotels
  3.5% MR/LWAL+CDL/H:1/Hotels
  7.1% MR/LWAL+CDL/H:2/Hotels
  25.1% MR/LWAL+CDL/HBET:3-5/Hotels
@@ -85,8 +101,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,10 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,6 +168,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -195,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,9 +254,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,6 +306,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,14 +499,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,14 +524,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="335" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Revert "update Gibraltar com typologies 50:50 CDL/CDN"""
This reverts commit f4b6f542f2115c773295a7b658a09046ffd1c8cf.
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
+++ b/com_mapping_schemes/mapping_Gibraltar_COM.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFF583B-EF5C-1F46-B7DC-B09CF39B435A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="20520" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -31,14 +25,10 @@
     <t>Hotels</t>
   </si>
   <si>
-    <t>1.8% CR/LFM+CDN/H:1/Offices
-4.55% CR/LFM+CDN/H:2/Offices
-10.9% CR/LFM+CDN/HBET:3-5/Offices
-0.9% CR/LFM+CDN/HBET:6-/Offices
-1.8% CR/LFM+CDL/H:1/Offices
-4.55% CR/LFM+CDL/H:2/Offices
-10.9% CR/LFM+CDL/HBET:3-5/Offices
-0.9% CR/LFM+CDL/HBET:6-/Offices
+    <t>3.6% CR/LFM+CDL/H:1/Offices
+9.1% CR/LFM+CDL/H:2/Offices
+21.8% CR/LFM+CDL/HBET:3-5/Offices
+1.8% CR/LFM+CDL/HBET:6-/Offices
 3.6% MR/LWAL+CDL/H:1/Offices
 7.3% MR/LWAL+CDL/H:2/Offices
 25.5% MR/LWAL+CDL/HBET:3-5/Offices
@@ -54,10 +44,8 @@
 0.0% W/LFM+CDL/H:2/Offices</t>
   </si>
   <si>
-    <t>8.2% CR/LFM+CDL/H:1/Trade
-0.9% CR/LFM+CDL/H:2/Trade
-8.2% CR/LFM+CDL/H:1/Trade
-0.9% CR/LFM+CDL/H:2/Trade
+    <t>16.4% CR/LFM+CDL/H:1/Trade
+1.8% CR/LFM+CDL/H:2/Trade
 0.0% CR/LFM+CDL/HBET:3-5/Trade
 0.0% CR/LFM+CDL/HBET:6-/Trade
 32.7% MR/LWAL+CDL/H:1/Trade
@@ -75,14 +63,10 @@
 0.4% W/LFM+CDL/H:2/Trade</t>
   </si>
   <si>
-    <t>2.2% CR/LFM+CDN/H:1/Hotels
-0.9% CR/LFM+CDN/H:2/Hotels
-5.3% CR/LFM+CDN/HBET:3-5/Hotels
-0.45% CR/LFM+CDN/HBET:6-/Hotels
-2.2% CR/LFM+CDL/H:1/Hotels
-0.9% CR/LFM+CDL/H:2/Hotels
-5.3% CR/LFM+CDL/HBET:3-5/Hotels
-0.45% CR/LFM+CDL/HBET:6-/Hotels
+    <t>4.4% CR/LFM+CDL/H:1/Hotels
+ 1.8% CR/LFM+CDL/H:2/Hotels
+ 10.6% CR/LFM+CDL/HBET:3-5/Hotels
+ 0.9% CR/LFM+CDL/HBET:6-/Hotels
  3.5% MR/LWAL+CDL/H:1/Hotels
  7.1% MR/LWAL+CDL/H:2/Hotels
  25.1% MR/LWAL+CDL/HBET:3-5/Hotels
@@ -101,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,13 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -168,14 +149,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -222,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,27 +227,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,24 +261,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,21 +436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,14 +454,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="335" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>